<commit_message>
[DATA] synspective data consistent formatting
</commit_message>
<xml_diff>
--- a/financial_data/synspective.xlsx
+++ b/financial_data/synspective.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AC832B-CAD0-4DD7-AA81-38EAFD72D2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14F5893-A96B-4AEA-8F19-9D384469E6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="income" sheetId="3" r:id="rId1"/>
+    <sheet name="consolidated" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -80,10 +80,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="165" formatCode="&quot;¥&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,8 +248,14 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,12 +433,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -596,19 +596,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -616,9 +607,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -977,916 +973,916 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C421C4D6-D1ED-2D45-BDB3-F7E485213868}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.5" style="1"/>
-    <col min="2" max="2" width="14.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.5" style="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.125" customWidth="1"/>
-    <col min="12" max="12" width="17.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" ht="28.5">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" ht="18.75">
-      <c r="A2" s="2">
+      <c r="A2" s="7">
         <v>43465</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>2002976</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>8955</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>2011932</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>54122</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <f>SUM(G2:I2)</f>
         <v>1957810</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>100000</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>2146200</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>-288390</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <v>0</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="8">
         <v>1957810</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="8">
         <f>E2+F2+J2</f>
         <v>2011932</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="18.75">
-      <c r="A3" s="3">
+      <c r="A3" s="7">
         <v>43555</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <f>(B2-B4)/($A4-$A2)*($A4-$A3)+B4</f>
         <v>3769019.1232876712</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <f>(C2-C4)/($A4-$A2)*($A4-$A3)+C4</f>
         <v>51645.821917808214</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <f t="shared" ref="D3:L15" si="0">(D2-D4)/($A4-$A2)*($A4-$A3)+D4</f>
         <v>3820665.6986301374</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <f t="shared" si="0"/>
         <v>59330.657534246573</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <f t="shared" si="0"/>
         <v>3761335.0410958901</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="8">
         <f t="shared" si="0"/>
         <v>4284040.5205479451</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <f t="shared" si="0"/>
         <v>-622705.47945205483</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="8">
         <f t="shared" ref="K3" si="1">(K2-K4)/($A4-$A2)*($A4-$A3)+K4</f>
         <v>3761335.0410958901</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="8">
         <f t="shared" si="0"/>
         <v>3820665.6986301374</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="18.75">
-      <c r="A4" s="5">
+      <c r="A4" s="7">
         <v>43646</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <f>(B2-B6)/($A6-$A2)*($A6-$A4)+B6</f>
         <v>5554684.9479452055</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <f>(C2-C6)/($A6-$A2)*($A6-$A4)+C6</f>
         <v>94810.986301369863</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <f t="shared" ref="D4:I4" si="2">(D2-D6)/($A6-$A2)*($A6-$A4)+D6</f>
         <v>5649496.4383561648</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <f t="shared" si="2"/>
         <v>64597.189041095888</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <f t="shared" ref="F4" si="3">(F2-F6)/($A6-$A2)*($A6-$A4)+F6</f>
         <v>5584899.2493150681</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="8">
         <f t="shared" si="2"/>
         <v>100000</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="8">
         <f t="shared" si="2"/>
         <v>6445634.8246575342</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <f t="shared" si="2"/>
         <v>-960735.57534246577</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="8">
         <f t="shared" ref="J4:K4" si="4">(J2-J6)/($A6-$A2)*($A6-$A4)+J6</f>
         <v>0</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="8">
         <f t="shared" si="4"/>
         <v>5584899.2493150681</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="8">
         <f t="shared" ref="L4" si="5">(L2-L6)/($A6-$A2)*($A6-$A4)+L6</f>
         <v>5649496.4383561648</v>
       </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="18.75">
-      <c r="A5" s="3">
+      <c r="A5" s="7">
         <v>43738</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="8">
         <f>(B4-B6)/($A6-$A4)*($A6-$A5)+B6</f>
         <v>7359973.4739726027</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <f>(C4-C6)/($A6-$A4)*($A6-$A5)+C6</f>
         <v>138450.49315068492</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <f t="shared" ref="D5:L5" si="6">(D4-D6)/($A6-$A4)*($A6-$A5)+D6</f>
         <v>7498424.2191780824</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <f t="shared" si="6"/>
         <v>69921.594520547951</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <f t="shared" si="6"/>
         <v>7428502.6246575341</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <f t="shared" si="6"/>
         <v>100000</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <f t="shared" si="6"/>
         <v>8630982.9123287667</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <f t="shared" si="6"/>
         <v>-1302480.2876712328</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="8">
         <f t="shared" ref="K5" si="7">(K4-K6)/($A6-$A4)*($A6-$A5)+K6</f>
         <v>7428502.6246575341</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="8">
         <f t="shared" si="6"/>
         <v>7498424.2191780824</v>
       </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="18.75">
-      <c r="A6" s="2">
+      <c r="A6" s="7">
         <v>43830</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>9165262</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>182090</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>9347352</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>75246</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <f>SUM(G6:I6)</f>
         <v>9272106</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>100000</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>10816331</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="8">
         <v>-1644225</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <v>0</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="8">
         <v>9272106</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="8">
         <f>E6+F6+J6</f>
         <v>9347352</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" ht="18.75">
-      <c r="A7" s="3">
+      <c r="A7" s="7">
         <v>43921</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <f>(B6-B8)/($A8-$A6)*($A8-$A7)+B8</f>
         <v>8509201.9754098356</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <f>(C6-C8)/($A8-$A6)*($A8-$A7)+C8</f>
         <v>187245.17486338798</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <f t="shared" ref="D7" si="8">(D6-D8)/($A8-$A6)*($A8-$A7)+D8</f>
         <v>8696447.3989071026</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <f t="shared" ref="E7:F7" si="9">(E6-E8)/($A8-$A6)*($A8-$A7)+E8</f>
         <v>95018.112021857931</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="8">
         <f t="shared" si="9"/>
         <v>8601149.5737704914</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="8">
         <f t="shared" ref="G7" si="10">(G6-G8)/($A8-$A6)*($A8-$A7)+G8</f>
         <v>100000</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="8">
         <f t="shared" ref="H7" si="11">(H6-H8)/($A8-$A6)*($A8-$A7)+H8</f>
         <v>10816331.24863388</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="8">
         <f t="shared" ref="I7" si="12">(I6-I8)/($A8-$A6)*($A8-$A7)+I8</f>
         <v>-2315181.4262295081</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="8">
         <f t="shared" si="0"/>
         <v>279.71311475409834</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="8">
         <f t="shared" si="0"/>
         <v>8601149.5737704914</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="8">
         <f t="shared" si="0"/>
         <v>8696447.3989071026</v>
       </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" ht="18.75">
-      <c r="A8" s="5">
+      <c r="A8" s="7">
         <v>44012</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <f>(B6-B10)/($A10-$A6)*($A10-$A8)+B10</f>
         <v>7853141.9508196721</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <f>(C6-C10)/($A10-$A6)*($A10-$A8)+C10</f>
         <v>192400.34972677595</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <f t="shared" ref="D8:L8" si="13">(D6-D10)/($A10-$A6)*($A10-$A8)+D10</f>
         <v>8045542.7978142072</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <f t="shared" si="13"/>
         <v>114790.22404371585</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <f t="shared" si="13"/>
         <v>7930193.1475409837</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="8">
         <f t="shared" si="13"/>
         <v>100000</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="8">
         <f t="shared" si="13"/>
         <v>10816331.49726776</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="8">
         <f t="shared" si="13"/>
         <v>-2986137.8524590163</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="8">
         <f t="shared" si="13"/>
         <v>559.42622950819668</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="8">
         <f t="shared" ref="K8" si="14">(K6-K10)/($A10-$A6)*($A10-$A8)+K10</f>
         <v>7930193.1475409837</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="8">
         <f t="shared" si="13"/>
         <v>8045542.7978142072</v>
       </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="18.75">
-      <c r="A9" s="3">
+      <c r="A9" s="7">
         <v>44104</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <f>(B8-B10)/($A10-$A8)*($A10-$A9)+B10</f>
         <v>7189872.4754098356</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <f>(C8-C10)/($A10-$A8)*($A10-$A9)+C10</f>
         <v>197612.17486338798</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <f t="shared" ref="D9" si="15">(D8-D10)/($A10-$A8)*($A10-$A9)+D10</f>
         <v>7387485.3989071036</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <f t="shared" ref="E9:F9" si="16">(E8-E10)/($A10-$A8)*($A10-$A9)+E10</f>
         <v>134779.61202185793</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <f t="shared" si="16"/>
         <v>7251863.5737704914</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="8">
         <f t="shared" ref="G9" si="17">(G8-G10)/($A10-$A8)*($A10-$A9)+G10</f>
         <v>100000</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="8">
         <f t="shared" ref="H9" si="18">(H8-H10)/($A10-$A8)*($A10-$A9)+H10</f>
         <v>10816331.74863388</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="8">
         <f t="shared" ref="I9:L9" si="19">(I8-I10)/($A10-$A8)*($A10-$A9)+I10</f>
         <v>-3664467.4262295081</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="8">
         <f t="shared" si="19"/>
         <v>842.21311475409834</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="8">
         <f t="shared" si="19"/>
         <v>7251863.5737704914</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="8">
         <f t="shared" si="19"/>
         <v>7387485.3989071036</v>
       </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" ht="18.75">
-      <c r="A10" s="2">
+      <c r="A10" s="7">
         <v>44196</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>6526603</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>202824</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>6729428</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>154769</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>6573534</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>100000</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>10816332</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>-4342797</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <v>1125</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="8">
         <v>6573534</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="8">
         <f>E10+F10+J10</f>
         <v>6729428</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:16" ht="18.75">
-      <c r="A11" s="3">
+      <c r="A11" s="7">
         <v>44286</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="8">
         <f>(B10-B12)/($A12-$A10)*($A12-$A11)+B12</f>
         <v>7054816.2054794524</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <f>(C10-C12)/($A12-$A10)*($A12-$A11)+C12</f>
         <v>268071.53424657538</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="8">
         <f t="shared" ref="D11" si="20">(D10-D12)/($A12-$A10)*($A12-$A11)+D12</f>
         <v>7322888.493150685</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="8">
         <f t="shared" ref="E11:F11" si="21">(E10-E12)/($A12-$A10)*($A12-$A11)+E12</f>
         <v>165132.56164383562</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <f t="shared" si="21"/>
         <v>7156630.6849315064</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="8">
         <f t="shared" ref="G11" si="22">(G10-G12)/($A12-$A10)*($A12-$A11)+G12</f>
         <v>100000</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="8">
         <f t="shared" ref="H11" si="23">(H10-H12)/($A12-$A10)*($A12-$A11)+H12</f>
         <v>12007327.890410958</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="8">
         <f t="shared" ref="I11" si="24">(I10-I12)/($A12-$A10)*($A12-$A11)+I12</f>
         <v>-4950696.2054794524</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="8">
         <f t="shared" si="0"/>
         <v>1125</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="8">
         <f t="shared" si="0"/>
         <v>7156630.6849315064</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="8">
         <f t="shared" si="0"/>
         <v>7322888.493150685</v>
       </c>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" ht="18.75">
-      <c r="A12" s="5">
+      <c r="A12" s="7">
         <v>44377</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="8">
         <f>(B10-B14)/($A14-$A10)*($A14-$A12)+B14</f>
         <v>7588898.4465753427</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="8">
         <f>(C10-C14)/($A14-$A10)*($A14-$A12)+C14</f>
         <v>334044.04109589045</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="8">
         <f t="shared" ref="D12:L12" si="25">(D10-D14)/($A14-$A10)*($A14-$A12)+D14</f>
         <v>7922942.9917808222</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="8">
         <f t="shared" si="25"/>
         <v>175611.27397260274</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="8">
         <f t="shared" si="25"/>
         <v>7746206.2219178081</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="8">
         <f t="shared" si="25"/>
         <v>100000</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="8">
         <f t="shared" si="25"/>
         <v>13211557.06849315</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="8">
         <f t="shared" si="25"/>
         <v>-5565349.8465753421</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="8">
         <f t="shared" si="25"/>
         <v>1125</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="8">
         <f t="shared" ref="K12" si="26">(K10-K14)/($A14-$A10)*($A14-$A12)+K14</f>
         <v>7746206.2219178081</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="8">
         <f t="shared" si="25"/>
         <v>7922942.9917808222</v>
       </c>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" ht="18.75">
-      <c r="A13" s="3">
+      <c r="A13" s="7">
         <v>44469</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="8">
         <f>(B12-B14)/($A14-$A12)*($A14-$A13)+B14</f>
         <v>8128849.7232876718</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="8">
         <f>(C12-C14)/($A14-$A12)*($A14-$A13)+C14</f>
         <v>400741.52054794523</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="8">
         <f t="shared" ref="D13" si="27">(D12-D14)/($A14-$A12)*($A14-$A13)+D14</f>
         <v>8529591.4958904106</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="8">
         <f t="shared" ref="E13:F13" si="28">(E12-E14)/($A14-$A12)*($A14-$A13)+E14</f>
         <v>186205.13698630137</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="8">
         <f t="shared" si="28"/>
         <v>8342260.610958904</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="8">
         <f t="shared" ref="G13" si="29">(G12-G14)/($A14-$A12)*($A14-$A13)+G14</f>
         <v>100000</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="8">
         <f t="shared" ref="H13" si="30">(H12-H14)/($A14-$A12)*($A14-$A13)+H14</f>
         <v>14429019.534246575</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="8">
         <f t="shared" ref="I13:L13" si="31">(I12-I14)/($A14-$A12)*($A14-$A13)+I14</f>
         <v>-6186757.9232876711</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="8">
         <f t="shared" si="31"/>
         <v>1125</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="8">
         <f t="shared" si="31"/>
         <v>8342260.610958904</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="8">
         <f t="shared" si="31"/>
         <v>8529591.4958904106</v>
       </c>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16" ht="18.75">
-      <c r="A14" s="2">
+      <c r="A14" s="7">
         <v>44561</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>8668801</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>467439</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>9136240</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>196799</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>8938315</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <v>100000</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>15646482</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="8">
         <v>-6808166</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <v>1125</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="8">
         <v>8938315</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="8">
         <v>9136240</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:16" ht="18.75">
-      <c r="A15" s="3">
+      <c r="A15" s="7">
         <v>44651</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="8">
         <f>(B14-B16)/($A16-$A14)*($A16-$A15)+B16</f>
         <v>8360675.2739726026</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="8">
         <f>(C14-C16)/($A16-$A14)*($A16-$A15)+C16</f>
         <v>973527.49315068498</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="8">
         <f t="shared" ref="D15" si="32">(D14-D16)/($A16-$A14)*($A16-$A15)+D16</f>
         <v>9334203.01369863</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="8">
         <f t="shared" ref="E15:F15" si="33">(E14-E16)/($A16-$A14)*($A16-$A15)+E16</f>
         <v>595718.94520547951</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="8">
         <f t="shared" si="33"/>
         <v>8737286.8082191776</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="8">
         <f t="shared" ref="G15" si="34">(G14-G16)/($A16-$A14)*($A16-$A15)+G16</f>
         <v>100000</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="8">
         <f t="shared" ref="H15" si="35">(H14-H16)/($A16-$A14)*($A16-$A15)+H16</f>
         <v>15311537.753424658</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="8">
         <f t="shared" ref="I15" si="36">(I14-I16)/($A16-$A14)*($A16-$A15)+I16</f>
         <v>-6674249.9452054799</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="8">
         <f t="shared" si="0"/>
         <v>1196.013698630137</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="8">
         <f t="shared" si="0"/>
         <v>8737286.8082191776</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="8">
         <f t="shared" si="0"/>
         <v>9334203.01369863</v>
       </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16" ht="18.75">
-      <c r="A16" s="5">
+      <c r="A16" s="7">
         <v>44742</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="8">
         <f>(B14-B18)/($A18-$A14)*($A18-$A16)+B18</f>
         <v>8049125.9287671233</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="8">
         <f>(C14-C18)/($A18-$A14)*($A18-$A16)+C18</f>
         <v>1485239.1917808219</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="8">
         <f t="shared" ref="D16:L16" si="37">(D14-D18)/($A18-$A14)*($A18-$A16)+D18</f>
         <v>9534365.6164383553</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <f t="shared" si="37"/>
         <v>999071.33424657537</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="8">
         <f t="shared" si="37"/>
         <v>8534024.9698630143</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="8">
         <f t="shared" si="37"/>
         <v>100000</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="8">
         <f t="shared" si="37"/>
         <v>14972871.90410959</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="8">
         <f t="shared" si="37"/>
         <v>-6538845.9342465755</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="8">
         <f t="shared" si="37"/>
         <v>1267.8164383561643</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="8">
         <f t="shared" ref="K16" si="38">(K14-K18)/($A18-$A14)*($A18-$A16)+K18</f>
         <v>8534024.9698630143</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="8">
         <f t="shared" si="37"/>
         <v>9534365.6164383553</v>
       </c>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16" ht="18.75">
-      <c r="A17" s="3">
+      <c r="A17" s="7">
         <v>44834</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="8">
         <f>(B16-B18)/($A18-$A16)*($A18-$A17)+B18</f>
         <v>7734152.9643835612</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="8">
         <f>(C16-C18)/($A18-$A16)*($A18-$A17)+C18</f>
         <v>2002574.0958904109</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="8">
         <f t="shared" ref="D17" si="39">(D16-D18)/($A18-$A16)*($A18-$A17)+D18</f>
         <v>9736727.8082191776</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="8">
         <f t="shared" ref="E17:F17" si="40">(E16-E18)/($A18-$A16)*($A18-$A17)+E18</f>
         <v>1406856.1671232877</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="8">
         <f t="shared" si="40"/>
         <v>8328529.4849315071</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="8">
         <f t="shared" ref="G17" si="41">(G16-G18)/($A18-$A16)*($A18-$A17)+G18</f>
         <v>100000</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="8">
         <f t="shared" ref="H17" si="42">(H16-H18)/($A18-$A16)*($A18-$A17)+H18</f>
         <v>14630484.452054795</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <f t="shared" ref="I17:L17" si="43">(I16-I18)/($A18-$A16)*($A18-$A17)+I18</f>
         <v>-6401953.9671232877</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="8">
         <f t="shared" si="43"/>
         <v>1340.4082191780822</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="8">
         <f t="shared" si="43"/>
         <v>8328529.4849315071</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="8">
         <f t="shared" si="43"/>
         <v>9736727.8082191776</v>
       </c>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16" ht="18.75">
-      <c r="A18" s="2">
+      <c r="A18" s="7">
         <v>44926</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>7419180</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>2519909</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>9939090</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>1814641</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>8123034</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>100000</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>14288097</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="8">
         <v>-6265062</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <v>1413</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="8">
         <v>8123034</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="8">
         <v>9939090</v>
       </c>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>

</xml_diff>

<commit_message>
[ADD] change '-' to '0' in synspective empty columns
</commit_message>
<xml_diff>
--- a/financial_data/synspective.xlsx
+++ b/financial_data/synspective.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14F5893-A96B-4AEA-8F19-9D384469E6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC40958D-054C-428F-8AE1-7A19460554DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,8 +80,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -610,12 +610,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -973,22 +971,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C421C4D6-D1ED-2D45-BDB3-F7E485213868}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1"/>
-    <col min="2" max="2" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
@@ -1051,7 +1050,6 @@
         <v>54122</v>
       </c>
       <c r="F2" s="8">
-        <f>SUM(G2:I2)</f>
         <v>1957810</v>
       </c>
       <c r="G2" s="8">
@@ -1070,7 +1068,6 @@
         <v>1957810</v>
       </c>
       <c r="L2" s="8">
-        <f>E2+F2+J2</f>
         <v>2011932</v>
       </c>
       <c r="M2" s="3"/>
@@ -1082,47 +1079,36 @@
         <v>43555</v>
       </c>
       <c r="B3" s="8">
-        <f>(B2-B4)/($A4-$A2)*($A4-$A3)+B4</f>
         <v>3769019.1232876712</v>
       </c>
       <c r="C3" s="8">
-        <f>(C2-C4)/($A4-$A2)*($A4-$A3)+C4</f>
         <v>51645.821917808214</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:L15" si="0">(D2-D4)/($A4-$A2)*($A4-$A3)+D4</f>
         <v>3820665.6986301374</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" si="0"/>
         <v>59330.657534246573</v>
       </c>
       <c r="F3" s="8">
-        <f t="shared" si="0"/>
         <v>3761335.0410958901</v>
       </c>
       <c r="G3" s="8">
-        <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" si="0"/>
         <v>4284040.5205479451</v>
       </c>
       <c r="I3" s="8">
-        <f t="shared" si="0"/>
         <v>-622705.47945205483</v>
       </c>
       <c r="J3" s="8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K3" s="8">
-        <f t="shared" ref="K3" si="1">(K2-K4)/($A4-$A2)*($A4-$A3)+K4</f>
         <v>3761335.0410958901</v>
       </c>
       <c r="L3" s="8">
-        <f t="shared" si="0"/>
         <v>3820665.6986301374</v>
       </c>
       <c r="M3" s="4"/>
@@ -1135,47 +1121,36 @@
         <v>43646</v>
       </c>
       <c r="B4" s="8">
-        <f>(B2-B6)/($A6-$A2)*($A6-$A4)+B6</f>
         <v>5554684.9479452055</v>
       </c>
       <c r="C4" s="8">
-        <f>(C2-C6)/($A6-$A2)*($A6-$A4)+C6</f>
         <v>94810.986301369863</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:I4" si="2">(D2-D6)/($A6-$A2)*($A6-$A4)+D6</f>
         <v>5649496.4383561648</v>
       </c>
       <c r="E4" s="8">
-        <f t="shared" si="2"/>
         <v>64597.189041095888</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" ref="F4" si="3">(F2-F6)/($A6-$A2)*($A6-$A4)+F6</f>
         <v>5584899.2493150681</v>
       </c>
       <c r="G4" s="8">
-        <f t="shared" si="2"/>
         <v>100000</v>
       </c>
       <c r="H4" s="8">
-        <f t="shared" si="2"/>
         <v>6445634.8246575342</v>
       </c>
       <c r="I4" s="8">
-        <f t="shared" si="2"/>
         <v>-960735.57534246577</v>
       </c>
       <c r="J4" s="8">
-        <f t="shared" ref="J4:K4" si="4">(J2-J6)/($A6-$A2)*($A6-$A4)+J6</f>
         <v>0</v>
       </c>
       <c r="K4" s="8">
-        <f t="shared" si="4"/>
         <v>5584899.2493150681</v>
       </c>
       <c r="L4" s="8">
-        <f t="shared" ref="L4" si="5">(L2-L6)/($A6-$A2)*($A6-$A4)+L6</f>
         <v>5649496.4383561648</v>
       </c>
       <c r="M4" s="4"/>
@@ -1188,47 +1163,36 @@
         <v>43738</v>
       </c>
       <c r="B5" s="8">
-        <f>(B4-B6)/($A6-$A4)*($A6-$A5)+B6</f>
         <v>7359973.4739726027</v>
       </c>
       <c r="C5" s="8">
-        <f>(C4-C6)/($A6-$A4)*($A6-$A5)+C6</f>
         <v>138450.49315068492</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" ref="D5:L5" si="6">(D4-D6)/($A6-$A4)*($A6-$A5)+D6</f>
         <v>7498424.2191780824</v>
       </c>
       <c r="E5" s="8">
-        <f t="shared" si="6"/>
         <v>69921.594520547951</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" si="6"/>
         <v>7428502.6246575341</v>
       </c>
       <c r="G5" s="8">
-        <f t="shared" si="6"/>
         <v>100000</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" si="6"/>
         <v>8630982.9123287667</v>
       </c>
       <c r="I5" s="8">
-        <f t="shared" si="6"/>
         <v>-1302480.2876712328</v>
       </c>
       <c r="J5" s="8">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K5" s="8">
-        <f t="shared" ref="K5" si="7">(K4-K6)/($A6-$A4)*($A6-$A5)+K6</f>
         <v>7428502.6246575341</v>
       </c>
       <c r="L5" s="8">
-        <f t="shared" si="6"/>
         <v>7498424.2191780824</v>
       </c>
       <c r="M5" s="4"/>
@@ -1253,7 +1217,6 @@
         <v>75246</v>
       </c>
       <c r="F6" s="8">
-        <f>SUM(G6:I6)</f>
         <v>9272106</v>
       </c>
       <c r="G6" s="8">
@@ -1272,7 +1235,6 @@
         <v>9272106</v>
       </c>
       <c r="L6" s="8">
-        <f>E6+F6+J6</f>
         <v>9347352</v>
       </c>
       <c r="M6" s="5"/>
@@ -1285,47 +1247,36 @@
         <v>43921</v>
       </c>
       <c r="B7" s="8">
-        <f>(B6-B8)/($A8-$A6)*($A8-$A7)+B8</f>
         <v>8509201.9754098356</v>
       </c>
       <c r="C7" s="8">
-        <f>(C6-C8)/($A8-$A6)*($A8-$A7)+C8</f>
         <v>187245.17486338798</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" ref="D7" si="8">(D6-D8)/($A8-$A6)*($A8-$A7)+D8</f>
         <v>8696447.3989071026</v>
       </c>
       <c r="E7" s="8">
-        <f t="shared" ref="E7:F7" si="9">(E6-E8)/($A8-$A6)*($A8-$A7)+E8</f>
         <v>95018.112021857931</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" si="9"/>
         <v>8601149.5737704914</v>
       </c>
       <c r="G7" s="8">
-        <f t="shared" ref="G7" si="10">(G6-G8)/($A8-$A6)*($A8-$A7)+G8</f>
         <v>100000</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" ref="H7" si="11">(H6-H8)/($A8-$A6)*($A8-$A7)+H8</f>
         <v>10816331.24863388</v>
       </c>
       <c r="I7" s="8">
-        <f t="shared" ref="I7" si="12">(I6-I8)/($A8-$A6)*($A8-$A7)+I8</f>
         <v>-2315181.4262295081</v>
       </c>
       <c r="J7" s="8">
-        <f t="shared" si="0"/>
         <v>279.71311475409834</v>
       </c>
       <c r="K7" s="8">
-        <f t="shared" si="0"/>
         <v>8601149.5737704914</v>
       </c>
       <c r="L7" s="8">
-        <f t="shared" si="0"/>
         <v>8696447.3989071026</v>
       </c>
       <c r="M7" s="4"/>
@@ -1338,47 +1289,36 @@
         <v>44012</v>
       </c>
       <c r="B8" s="8">
-        <f>(B6-B10)/($A10-$A6)*($A10-$A8)+B10</f>
         <v>7853141.9508196721</v>
       </c>
       <c r="C8" s="8">
-        <f>(C6-C10)/($A10-$A6)*($A10-$A8)+C10</f>
         <v>192400.34972677595</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" ref="D8:L8" si="13">(D6-D10)/($A10-$A6)*($A10-$A8)+D10</f>
         <v>8045542.7978142072</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" si="13"/>
         <v>114790.22404371585</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="13"/>
         <v>7930193.1475409837</v>
       </c>
       <c r="G8" s="8">
-        <f t="shared" si="13"/>
         <v>100000</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="13"/>
         <v>10816331.49726776</v>
       </c>
       <c r="I8" s="8">
-        <f t="shared" si="13"/>
         <v>-2986137.8524590163</v>
       </c>
       <c r="J8" s="8">
-        <f t="shared" si="13"/>
         <v>559.42622950819668</v>
       </c>
       <c r="K8" s="8">
-        <f t="shared" ref="K8" si="14">(K6-K10)/($A10-$A6)*($A10-$A8)+K10</f>
         <v>7930193.1475409837</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="13"/>
         <v>8045542.7978142072</v>
       </c>
       <c r="M8" s="4"/>
@@ -1391,47 +1331,36 @@
         <v>44104</v>
       </c>
       <c r="B9" s="8">
-        <f>(B8-B10)/($A10-$A8)*($A10-$A9)+B10</f>
         <v>7189872.4754098356</v>
       </c>
       <c r="C9" s="8">
-        <f>(C8-C10)/($A10-$A8)*($A10-$A9)+C10</f>
         <v>197612.17486338798</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" ref="D9" si="15">(D8-D10)/($A10-$A8)*($A10-$A9)+D10</f>
         <v>7387485.3989071036</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" ref="E9:F9" si="16">(E8-E10)/($A10-$A8)*($A10-$A9)+E10</f>
         <v>134779.61202185793</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="16"/>
         <v>7251863.5737704914</v>
       </c>
       <c r="G9" s="8">
-        <f t="shared" ref="G9" si="17">(G8-G10)/($A10-$A8)*($A10-$A9)+G10</f>
         <v>100000</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" ref="H9" si="18">(H8-H10)/($A10-$A8)*($A10-$A9)+H10</f>
         <v>10816331.74863388</v>
       </c>
       <c r="I9" s="8">
-        <f t="shared" ref="I9:L9" si="19">(I8-I10)/($A10-$A8)*($A10-$A9)+I10</f>
         <v>-3664467.4262295081</v>
       </c>
       <c r="J9" s="8">
-        <f t="shared" si="19"/>
         <v>842.21311475409834</v>
       </c>
       <c r="K9" s="8">
-        <f t="shared" si="19"/>
         <v>7251863.5737704914</v>
       </c>
       <c r="L9" s="8">
-        <f t="shared" si="19"/>
         <v>7387485.3989071036</v>
       </c>
       <c r="M9" s="4"/>
@@ -1474,7 +1403,6 @@
         <v>6573534</v>
       </c>
       <c r="L10" s="8">
-        <f>E10+F10+J10</f>
         <v>6729428</v>
       </c>
       <c r="M10" s="5"/>
@@ -1487,47 +1415,36 @@
         <v>44286</v>
       </c>
       <c r="B11" s="8">
-        <f>(B10-B12)/($A12-$A10)*($A12-$A11)+B12</f>
         <v>7054816.2054794524</v>
       </c>
       <c r="C11" s="8">
-        <f>(C10-C12)/($A12-$A10)*($A12-$A11)+C12</f>
         <v>268071.53424657538</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" ref="D11" si="20">(D10-D12)/($A12-$A10)*($A12-$A11)+D12</f>
         <v>7322888.493150685</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" ref="E11:F11" si="21">(E10-E12)/($A12-$A10)*($A12-$A11)+E12</f>
         <v>165132.56164383562</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="21"/>
         <v>7156630.6849315064</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" ref="G11" si="22">(G10-G12)/($A12-$A10)*($A12-$A11)+G12</f>
         <v>100000</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" ref="H11" si="23">(H10-H12)/($A12-$A10)*($A12-$A11)+H12</f>
         <v>12007327.890410958</v>
       </c>
       <c r="I11" s="8">
-        <f t="shared" ref="I11" si="24">(I10-I12)/($A12-$A10)*($A12-$A11)+I12</f>
         <v>-4950696.2054794524</v>
       </c>
       <c r="J11" s="8">
-        <f t="shared" si="0"/>
         <v>1125</v>
       </c>
       <c r="K11" s="8">
-        <f t="shared" si="0"/>
         <v>7156630.6849315064</v>
       </c>
       <c r="L11" s="8">
-        <f t="shared" si="0"/>
         <v>7322888.493150685</v>
       </c>
       <c r="M11" s="4"/>
@@ -1540,47 +1457,36 @@
         <v>44377</v>
       </c>
       <c r="B12" s="8">
-        <f>(B10-B14)/($A14-$A10)*($A14-$A12)+B14</f>
         <v>7588898.4465753427</v>
       </c>
       <c r="C12" s="8">
-        <f>(C10-C14)/($A14-$A10)*($A14-$A12)+C14</f>
         <v>334044.04109589045</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" ref="D12:L12" si="25">(D10-D14)/($A14-$A10)*($A14-$A12)+D14</f>
         <v>7922942.9917808222</v>
       </c>
       <c r="E12" s="8">
-        <f t="shared" si="25"/>
         <v>175611.27397260274</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="25"/>
         <v>7746206.2219178081</v>
       </c>
       <c r="G12" s="8">
-        <f t="shared" si="25"/>
         <v>100000</v>
       </c>
       <c r="H12" s="8">
-        <f t="shared" si="25"/>
         <v>13211557.06849315</v>
       </c>
       <c r="I12" s="8">
-        <f t="shared" si="25"/>
         <v>-5565349.8465753421</v>
       </c>
       <c r="J12" s="8">
-        <f t="shared" si="25"/>
         <v>1125</v>
       </c>
       <c r="K12" s="8">
-        <f t="shared" ref="K12" si="26">(K10-K14)/($A14-$A10)*($A14-$A12)+K14</f>
         <v>7746206.2219178081</v>
       </c>
       <c r="L12" s="8">
-        <f t="shared" si="25"/>
         <v>7922942.9917808222</v>
       </c>
       <c r="M12" s="4"/>
@@ -1593,47 +1499,36 @@
         <v>44469</v>
       </c>
       <c r="B13" s="8">
-        <f>(B12-B14)/($A14-$A12)*($A14-$A13)+B14</f>
         <v>8128849.7232876718</v>
       </c>
       <c r="C13" s="8">
-        <f>(C12-C14)/($A14-$A12)*($A14-$A13)+C14</f>
         <v>400741.52054794523</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" ref="D13" si="27">(D12-D14)/($A14-$A12)*($A14-$A13)+D14</f>
         <v>8529591.4958904106</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" ref="E13:F13" si="28">(E12-E14)/($A14-$A12)*($A14-$A13)+E14</f>
         <v>186205.13698630137</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="28"/>
         <v>8342260.610958904</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" ref="G13" si="29">(G12-G14)/($A14-$A12)*($A14-$A13)+G14</f>
         <v>100000</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" ref="H13" si="30">(H12-H14)/($A14-$A12)*($A14-$A13)+H14</f>
         <v>14429019.534246575</v>
       </c>
       <c r="I13" s="8">
-        <f t="shared" ref="I13:L13" si="31">(I12-I14)/($A14-$A12)*($A14-$A13)+I14</f>
         <v>-6186757.9232876711</v>
       </c>
       <c r="J13" s="8">
-        <f t="shared" si="31"/>
         <v>1125</v>
       </c>
       <c r="K13" s="8">
-        <f t="shared" si="31"/>
         <v>8342260.610958904</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" si="31"/>
         <v>8529591.4958904106</v>
       </c>
       <c r="M13" s="4"/>
@@ -1688,47 +1583,36 @@
         <v>44651</v>
       </c>
       <c r="B15" s="8">
-        <f>(B14-B16)/($A16-$A14)*($A16-$A15)+B16</f>
         <v>8360675.2739726026</v>
       </c>
       <c r="C15" s="8">
-        <f>(C14-C16)/($A16-$A14)*($A16-$A15)+C16</f>
         <v>973527.49315068498</v>
       </c>
       <c r="D15" s="8">
-        <f t="shared" ref="D15" si="32">(D14-D16)/($A16-$A14)*($A16-$A15)+D16</f>
         <v>9334203.01369863</v>
       </c>
       <c r="E15" s="8">
-        <f t="shared" ref="E15:F15" si="33">(E14-E16)/($A16-$A14)*($A16-$A15)+E16</f>
         <v>595718.94520547951</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="33"/>
         <v>8737286.8082191776</v>
       </c>
       <c r="G15" s="8">
-        <f t="shared" ref="G15" si="34">(G14-G16)/($A16-$A14)*($A16-$A15)+G16</f>
         <v>100000</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" ref="H15" si="35">(H14-H16)/($A16-$A14)*($A16-$A15)+H16</f>
         <v>15311537.753424658</v>
       </c>
       <c r="I15" s="8">
-        <f t="shared" ref="I15" si="36">(I14-I16)/($A16-$A14)*($A16-$A15)+I16</f>
         <v>-6674249.9452054799</v>
       </c>
       <c r="J15" s="8">
-        <f t="shared" si="0"/>
         <v>1196.013698630137</v>
       </c>
       <c r="K15" s="8">
-        <f t="shared" si="0"/>
         <v>8737286.8082191776</v>
       </c>
       <c r="L15" s="8">
-        <f t="shared" si="0"/>
         <v>9334203.01369863</v>
       </c>
       <c r="M15" s="4"/>
@@ -1741,47 +1625,36 @@
         <v>44742</v>
       </c>
       <c r="B16" s="8">
-        <f>(B14-B18)/($A18-$A14)*($A18-$A16)+B18</f>
         <v>8049125.9287671233</v>
       </c>
       <c r="C16" s="8">
-        <f>(C14-C18)/($A18-$A14)*($A18-$A16)+C18</f>
         <v>1485239.1917808219</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" ref="D16:L16" si="37">(D14-D18)/($A18-$A14)*($A18-$A16)+D18</f>
         <v>9534365.6164383553</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="37"/>
         <v>999071.33424657537</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="37"/>
         <v>8534024.9698630143</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="37"/>
         <v>100000</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="37"/>
         <v>14972871.90410959</v>
       </c>
       <c r="I16" s="8">
-        <f t="shared" si="37"/>
         <v>-6538845.9342465755</v>
       </c>
       <c r="J16" s="8">
-        <f t="shared" si="37"/>
         <v>1267.8164383561643</v>
       </c>
       <c r="K16" s="8">
-        <f t="shared" ref="K16" si="38">(K14-K18)/($A18-$A14)*($A18-$A16)+K18</f>
         <v>8534024.9698630143</v>
       </c>
       <c r="L16" s="8">
-        <f t="shared" si="37"/>
         <v>9534365.6164383553</v>
       </c>
       <c r="M16" s="4"/>
@@ -1794,47 +1667,36 @@
         <v>44834</v>
       </c>
       <c r="B17" s="8">
-        <f>(B16-B18)/($A18-$A16)*($A18-$A17)+B18</f>
         <v>7734152.9643835612</v>
       </c>
       <c r="C17" s="8">
-        <f>(C16-C18)/($A18-$A16)*($A18-$A17)+C18</f>
         <v>2002574.0958904109</v>
       </c>
       <c r="D17" s="8">
-        <f t="shared" ref="D17" si="39">(D16-D18)/($A18-$A16)*($A18-$A17)+D18</f>
         <v>9736727.8082191776</v>
       </c>
       <c r="E17" s="8">
-        <f t="shared" ref="E17:F17" si="40">(E16-E18)/($A18-$A16)*($A18-$A17)+E18</f>
         <v>1406856.1671232877</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" si="40"/>
         <v>8328529.4849315071</v>
       </c>
       <c r="G17" s="8">
-        <f t="shared" ref="G17" si="41">(G16-G18)/($A18-$A16)*($A18-$A17)+G18</f>
         <v>100000</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" ref="H17" si="42">(H16-H18)/($A18-$A16)*($A18-$A17)+H18</f>
         <v>14630484.452054795</v>
       </c>
       <c r="I17" s="8">
-        <f t="shared" ref="I17:L17" si="43">(I16-I18)/($A18-$A16)*($A18-$A17)+I18</f>
         <v>-6401953.9671232877</v>
       </c>
       <c r="J17" s="8">
-        <f t="shared" si="43"/>
         <v>1340.4082191780822</v>
       </c>
       <c r="K17" s="8">
-        <f t="shared" si="43"/>
         <v>8328529.4849315071</v>
       </c>
       <c r="L17" s="8">
-        <f t="shared" si="43"/>
         <v>9736727.8082191776</v>
       </c>
       <c r="M17" s="4"/>

</xml_diff>

<commit_message>
[FIX] extra ghost columns in synspective data
</commit_message>
<xml_diff>
--- a/financial_data/synspective.xlsx
+++ b/financial_data/synspective.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC40958D-054C-428F-8AE1-7A19460554DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A495AC-2771-4ABF-AE31-E83C39A62D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="_-[$¥-411]* #,##0_-;\-[$¥-411]* #,##0_-;_-[$¥-411]* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -232,21 +232,6 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="11"/>
@@ -596,24 +581,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -969,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C421C4D6-D1ED-2D45-BDB3-F7E485213868}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
@@ -991,760 +968,689 @@
     <col min="13" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" ht="28.5">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" ht="18.75">
-      <c r="A2" s="7">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3">
         <v>43465</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="4">
         <v>2002976</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="4">
         <v>8955</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="4">
         <v>2011932</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="4">
         <v>54122</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="4">
         <v>1957810</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="4">
         <v>100000</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="4">
         <v>2146200</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="4">
         <v>-288390</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="4">
         <v>0</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="4">
         <v>1957810</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="4">
         <v>2011932</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" ht="18.75">
-      <c r="A3" s="7">
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="3">
         <v>43555</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>3769019.1232876712</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>51645.821917808214</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="4">
         <v>3820665.6986301374</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>59330.657534246573</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="4">
         <v>3761335.0410958901</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="4">
         <v>100000</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="4">
         <v>4284040.5205479451</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="4">
         <v>-622705.47945205483</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="4">
         <v>0</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="4">
         <v>3761335.0410958901</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="4">
         <v>3820665.6986301374</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" ht="18.75">
-      <c r="A4" s="7">
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="3">
         <v>43646</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="4">
         <v>5554684.9479452055</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="4">
         <v>94810.986301369863</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>5649496.4383561648</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>64597.189041095888</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="4">
         <v>5584899.2493150681</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="4">
         <v>100000</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="4">
         <v>6445634.8246575342</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="4">
         <v>-960735.57534246577</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="4">
         <v>0</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="4">
         <v>5584899.2493150681</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="4">
         <v>5649496.4383561648</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" ht="18.75">
-      <c r="A5" s="7">
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="3">
         <v>43738</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>7359973.4739726027</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>138450.49315068492</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>7498424.2191780824</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>69921.594520547951</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="4">
         <v>7428502.6246575341</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="4">
         <v>100000</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="4">
         <v>8630982.9123287667</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="4">
         <v>-1302480.2876712328</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="4">
         <v>7428502.6246575341</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="4">
         <v>7498424.2191780824</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75">
-      <c r="A6" s="7">
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3">
         <v>43830</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>9165262</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="4">
         <v>182090</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>9347352</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>75246</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="4">
         <v>9272106</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="4">
         <v>100000</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="4">
         <v>10816331</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="4">
         <v>-1644225</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="4">
         <v>0</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="4">
         <v>9272106</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="4">
         <v>9347352</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" ht="18.75">
-      <c r="A7" s="7">
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3">
         <v>43921</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>8509201.9754098356</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="4">
         <v>187245.17486338798</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>8696447.3989071026</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>95018.112021857931</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="4">
         <v>8601149.5737704914</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="4">
         <v>100000</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="4">
         <v>10816331.24863388</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="4">
         <v>-2315181.4262295081</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="4">
         <v>279.71311475409834</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="4">
         <v>8601149.5737704914</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="4">
         <v>8696447.3989071026</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="18.75">
-      <c r="A8" s="7">
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3">
         <v>44012</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="4">
         <v>7853141.9508196721</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="4">
         <v>192400.34972677595</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="4">
         <v>8045542.7978142072</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="4">
         <v>114790.22404371585</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="4">
         <v>7930193.1475409837</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="4">
         <v>100000</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="4">
         <v>10816331.49726776</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="4">
         <v>-2986137.8524590163</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="4">
         <v>559.42622950819668</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="4">
         <v>7930193.1475409837</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="4">
         <v>8045542.7978142072</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" ht="18.75">
-      <c r="A9" s="7">
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3">
         <v>44104</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="4">
         <v>7189872.4754098356</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="4">
         <v>197612.17486338798</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="4">
         <v>7387485.3989071036</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>134779.61202185793</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="4">
         <v>7251863.5737704914</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="4">
         <v>100000</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="4">
         <v>10816331.74863388</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="4">
         <v>-3664467.4262295081</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="4">
         <v>842.21311475409834</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="4">
         <v>7251863.5737704914</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="4">
         <v>7387485.3989071036</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" ht="18.75">
-      <c r="A10" s="7">
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3">
         <v>44196</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="4">
         <v>6526603</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="4">
         <v>202824</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="4">
         <v>6729428</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>154769</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="4">
         <v>6573534</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="4">
         <v>100000</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="4">
         <v>10816332</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="4">
         <v>-4342797</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="4">
         <v>1125</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="4">
         <v>6573534</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="4">
         <v>6729428</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" ht="18.75">
-      <c r="A11" s="7">
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3">
         <v>44286</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="4">
         <v>7054816.2054794524</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="4">
         <v>268071.53424657538</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="4">
         <v>7322888.493150685</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>165132.56164383562</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="4">
         <v>7156630.6849315064</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="4">
         <v>100000</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="4">
         <v>12007327.890410958</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="4">
         <v>-4950696.2054794524</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="4">
         <v>1125</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="4">
         <v>7156630.6849315064</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="4">
         <v>7322888.493150685</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" ht="18.75">
-      <c r="A12" s="7">
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3">
         <v>44377</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="4">
         <v>7588898.4465753427</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="4">
         <v>334044.04109589045</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="4">
         <v>7922942.9917808222</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>175611.27397260274</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="4">
         <v>7746206.2219178081</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="4">
         <v>100000</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="4">
         <v>13211557.06849315</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="4">
         <v>-5565349.8465753421</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="4">
         <v>1125</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="4">
         <v>7746206.2219178081</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="4">
         <v>7922942.9917808222</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" ht="18.75">
-      <c r="A13" s="7">
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3">
         <v>44469</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="4">
         <v>8128849.7232876718</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="4">
         <v>400741.52054794523</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="4">
         <v>8529591.4958904106</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>186205.13698630137</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="4">
         <v>8342260.610958904</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="4">
         <v>100000</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="4">
         <v>14429019.534246575</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="4">
         <v>-6186757.9232876711</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="4">
         <v>1125</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="4">
         <v>8342260.610958904</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="4">
         <v>8529591.4958904106</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" ht="18.75">
-      <c r="A14" s="7">
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3">
         <v>44561</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="4">
         <v>8668801</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="4">
         <v>467439</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="4">
         <v>9136240</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>196799</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="4">
         <v>8938315</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="4">
         <v>100000</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="4">
         <v>15646482</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="4">
         <v>-6808166</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="4">
         <v>1125</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="4">
         <v>8938315</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="4">
         <v>9136240</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" ht="18.75">
-      <c r="A15" s="7">
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3">
         <v>44651</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="4">
         <v>8360675.2739726026</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="4">
         <v>973527.49315068498</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="4">
         <v>9334203.01369863</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="4">
         <v>595718.94520547951</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="4">
         <v>8737286.8082191776</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="4">
         <v>100000</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="4">
         <v>15311537.753424658</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="4">
         <v>-6674249.9452054799</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="4">
         <v>1196.013698630137</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="4">
         <v>8737286.8082191776</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="4">
         <v>9334203.01369863</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" ht="18.75">
-      <c r="A16" s="7">
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3">
         <v>44742</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="4">
         <v>8049125.9287671233</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="4">
         <v>1485239.1917808219</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="4">
         <v>9534365.6164383553</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="4">
         <v>999071.33424657537</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="4">
         <v>8534024.9698630143</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="4">
         <v>100000</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="4">
         <v>14972871.90410959</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="4">
         <v>-6538845.9342465755</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="4">
         <v>1267.8164383561643</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="4">
         <v>8534024.9698630143</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="4">
         <v>9534365.6164383553</v>
       </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="1:16" ht="18.75">
-      <c r="A17" s="7">
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="3">
         <v>44834</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="4">
         <v>7734152.9643835612</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="4">
         <v>2002574.0958904109</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="4">
         <v>9736727.8082191776</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="4">
         <v>1406856.1671232877</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="4">
         <v>8328529.4849315071</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="4">
         <v>100000</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="4">
         <v>14630484.452054795</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="4">
         <v>-6401953.9671232877</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="4">
         <v>1340.4082191780822</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="4">
         <v>8328529.4849315071</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="4">
         <v>9736727.8082191776</v>
       </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="1:16" ht="18.75">
-      <c r="A18" s="7">
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="3">
         <v>44926</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="4">
         <v>7419180</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="4">
         <v>2519909</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="4">
         <v>9939090</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="4">
         <v>1814641</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="4">
         <v>8123034</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="4">
         <v>100000</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="4">
         <v>14288097</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="4">
         <v>-6265062</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="4">
         <v>1413</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="4">
         <v>8123034</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="4">
         <v>9939090</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>

</xml_diff>

<commit_message>
synspective FY2023 data added
</commit_message>
<xml_diff>
--- a/financial_data/synspective.xlsx
+++ b/financial_data/synspective.xlsx
@@ -1,13 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shinten/Desktop/untitled folder 3/space_econometrics/financial_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A260780-37C3-334E-A782-1721B5F251AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="3400" yWindow="500" windowWidth="19700" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="consolidated" sheetId="1" r:id="rId4"/>
+    <sheet name="consolidated" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FMl+/G/ikYw5Wy2lQadQXI4Ba7K5Elt5xuOoZPdboQM="/>
     </ext>
@@ -60,32 +80,37 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0_);\(&quot;¥&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="[$¥]#,##0"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,52 +118,64 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="5" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="5" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -328,34 +365,38 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:M22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="11.71"/>
-    <col customWidth="1" min="3" max="3" width="18.0"/>
-    <col customWidth="1" min="4" max="5" width="12.29"/>
-    <col customWidth="1" min="6" max="6" width="12.86"/>
-    <col customWidth="1" min="7" max="7" width="12.29"/>
-    <col customWidth="1" min="8" max="8" width="11.86"/>
-    <col customWidth="1" min="9" max="9" width="13.71"/>
-    <col customWidth="1" min="10" max="10" width="16.14"/>
-    <col customWidth="1" min="11" max="11" width="14.71"/>
-    <col customWidth="1" min="12" max="12" width="12.29"/>
-    <col customWidth="1" min="13" max="13" width="17.71"/>
+    <col min="1" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,53 +437,53 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43465.0</v>
+        <v>43465</v>
       </c>
       <c r="B2" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>2002976.0</v>
+        <v>2002976</v>
       </c>
       <c r="D2" s="5">
-        <v>8955.0</v>
+        <v>8955</v>
       </c>
       <c r="E2" s="5">
-        <v>2011932.0</v>
+        <v>2011932</v>
       </c>
       <c r="F2" s="5">
-        <v>54122.0</v>
+        <v>54122</v>
       </c>
       <c r="G2" s="5">
-        <v>1957810.0</v>
+        <v>1957810</v>
       </c>
       <c r="H2" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I2" s="5">
-        <v>2146200.0</v>
+        <v>2146200</v>
       </c>
       <c r="J2" s="5">
-        <v>-288390.0</v>
+        <v>-288390</v>
       </c>
       <c r="K2" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L2" s="5">
-        <v>1957810.0</v>
+        <v>1957810</v>
       </c>
       <c r="M2" s="5">
-        <v>2011932.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2011932</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43555.0</v>
+        <v>43555</v>
       </c>
       <c r="B3" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5">
         <v>3769019.1232876712</v>
@@ -454,329 +495,329 @@
         <v>3820665.6986301374</v>
       </c>
       <c r="F3" s="5">
-        <v>59330.65753424657</v>
+        <v>59330.657534246573</v>
       </c>
       <c r="G3" s="5">
-        <v>3761335.04109589</v>
+        <v>3761335.0410958901</v>
       </c>
       <c r="H3" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I3" s="5">
-        <v>4284040.520547945</v>
+        <v>4284040.5205479451</v>
       </c>
       <c r="J3" s="5">
-        <v>-622705.4794520548</v>
+        <v>-622705.47945205483</v>
       </c>
       <c r="K3" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L3" s="5">
-        <v>3761335.04109589</v>
+        <v>3761335.0410958901</v>
       </c>
       <c r="M3" s="5">
         <v>3820665.6986301374</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43646.0</v>
+        <v>43646</v>
       </c>
       <c r="B4" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
         <v>5554684.9479452055</v>
       </c>
       <c r="D4" s="5">
-        <v>94810.98630136986</v>
+        <v>94810.986301369863</v>
       </c>
       <c r="E4" s="5">
-        <v>5649496.438356165</v>
+        <v>5649496.4383561648</v>
       </c>
       <c r="F4" s="5">
-        <v>64597.18904109589</v>
+        <v>64597.189041095888</v>
       </c>
       <c r="G4" s="5">
-        <v>5584899.249315068</v>
+        <v>5584899.2493150681</v>
       </c>
       <c r="H4" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I4" s="5">
-        <v>6445634.824657534</v>
+        <v>6445634.8246575342</v>
       </c>
       <c r="J4" s="5">
-        <v>-960735.5753424658</v>
+        <v>-960735.57534246577</v>
       </c>
       <c r="K4" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L4" s="5">
-        <v>5584899.249315068</v>
+        <v>5584899.2493150681</v>
       </c>
       <c r="M4" s="5">
-        <v>5649496.438356165</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>5649496.4383561648</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43738.0</v>
+        <v>43738</v>
       </c>
       <c r="B5" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5">
-        <v>7359973.473972603</v>
+        <v>7359973.4739726027</v>
       </c>
       <c r="D5" s="5">
         <v>138450.49315068492</v>
       </c>
       <c r="E5" s="5">
-        <v>7498424.219178082</v>
+        <v>7498424.2191780824</v>
       </c>
       <c r="F5" s="5">
-        <v>69921.59452054795</v>
+        <v>69921.594520547951</v>
       </c>
       <c r="G5" s="5">
-        <v>7428502.624657534</v>
+        <v>7428502.6246575341</v>
       </c>
       <c r="H5" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I5" s="5">
-        <v>8630982.912328767</v>
+        <v>8630982.9123287667</v>
       </c>
       <c r="J5" s="5">
         <v>-1302480.2876712328</v>
       </c>
       <c r="K5" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L5" s="5">
-        <v>7428502.624657534</v>
+        <v>7428502.6246575341</v>
       </c>
       <c r="M5" s="5">
-        <v>7498424.219178082</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>7498424.2191780824</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43830.0</v>
+        <v>43830</v>
       </c>
       <c r="B6" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C6" s="5">
-        <v>9165262.0</v>
+        <v>9165262</v>
       </c>
       <c r="D6" s="5">
-        <v>182090.0</v>
+        <v>182090</v>
       </c>
       <c r="E6" s="5">
-        <v>9347352.0</v>
+        <v>9347352</v>
       </c>
       <c r="F6" s="5">
-        <v>75246.0</v>
+        <v>75246</v>
       </c>
       <c r="G6" s="5">
-        <v>9272106.0</v>
+        <v>9272106</v>
       </c>
       <c r="H6" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I6" s="5">
-        <v>1.0816331E7</v>
+        <v>10816331</v>
       </c>
       <c r="J6" s="5">
-        <v>-1644225.0</v>
+        <v>-1644225</v>
       </c>
       <c r="K6" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L6" s="5">
-        <v>9272106.0</v>
+        <v>9272106</v>
       </c>
       <c r="M6" s="5">
-        <v>9347352.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>9347352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43921.0</v>
+        <v>43921</v>
       </c>
       <c r="B7" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>8509201.975409836</v>
+        <v>8509201.9754098356</v>
       </c>
       <c r="D7" s="5">
         <v>187245.17486338798</v>
       </c>
       <c r="E7" s="5">
-        <v>8696447.398907103</v>
+        <v>8696447.3989071026</v>
       </c>
       <c r="F7" s="5">
-        <v>95018.11202185793</v>
+        <v>95018.112021857931</v>
       </c>
       <c r="G7" s="5">
-        <v>8601149.573770491</v>
+        <v>8601149.5737704914</v>
       </c>
       <c r="H7" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I7" s="5">
-        <v>1.081633124863388E7</v>
+        <v>10816331.24863388</v>
       </c>
       <c r="J7" s="5">
-        <v>-2315181.426229508</v>
+        <v>-2315181.4262295081</v>
       </c>
       <c r="K7" s="5">
         <v>279.71311475409834</v>
       </c>
       <c r="L7" s="5">
-        <v>8601149.573770491</v>
+        <v>8601149.5737704914</v>
       </c>
       <c r="M7" s="5">
-        <v>8696447.398907103</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>8696447.3989071026</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44012.0</v>
+        <v>44012</v>
       </c>
       <c r="B8" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5">
-        <v>7853141.950819672</v>
+        <v>7853141.9508196721</v>
       </c>
       <c r="D8" s="5">
         <v>192400.34972677595</v>
       </c>
       <c r="E8" s="5">
-        <v>8045542.797814207</v>
+        <v>8045542.7978142072</v>
       </c>
       <c r="F8" s="5">
         <v>114790.22404371585</v>
       </c>
       <c r="G8" s="5">
-        <v>7930193.147540984</v>
+        <v>7930193.1475409837</v>
       </c>
       <c r="H8" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I8" s="5">
-        <v>1.081633149726776E7</v>
+        <v>10816331.49726776</v>
       </c>
       <c r="J8" s="5">
         <v>-2986137.8524590163</v>
       </c>
       <c r="K8" s="5">
-        <v>559.4262295081967</v>
+        <v>559.42622950819668</v>
       </c>
       <c r="L8" s="5">
-        <v>7930193.147540984</v>
+        <v>7930193.1475409837</v>
       </c>
       <c r="M8" s="5">
-        <v>8045542.797814207</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>8045542.7978142072</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44104.0</v>
+        <v>44104</v>
       </c>
       <c r="B9" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C9" s="5">
-        <v>7189872.475409836</v>
+        <v>7189872.4754098356</v>
       </c>
       <c r="D9" s="5">
         <v>197612.17486338798</v>
       </c>
       <c r="E9" s="5">
-        <v>7387485.398907104</v>
+        <v>7387485.3989071036</v>
       </c>
       <c r="F9" s="5">
         <v>134779.61202185793</v>
       </c>
       <c r="G9" s="5">
-        <v>7251863.573770491</v>
+        <v>7251863.5737704914</v>
       </c>
       <c r="H9" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I9" s="5">
-        <v>1.081633174863388E7</v>
+        <v>10816331.74863388</v>
       </c>
       <c r="J9" s="5">
-        <v>-3664467.426229508</v>
+        <v>-3664467.4262295081</v>
       </c>
       <c r="K9" s="5">
-        <v>842.2131147540983</v>
+        <v>842.21311475409834</v>
       </c>
       <c r="L9" s="5">
-        <v>7251863.573770491</v>
+        <v>7251863.5737704914</v>
       </c>
       <c r="M9" s="5">
-        <v>7387485.398907104</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>7387485.3989071036</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44196.0</v>
+        <v>44196</v>
       </c>
       <c r="B10" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5">
-        <v>6526603.0</v>
+        <v>6526603</v>
       </c>
       <c r="D10" s="5">
-        <v>202824.0</v>
+        <v>202824</v>
       </c>
       <c r="E10" s="5">
-        <v>6729428.0</v>
+        <v>6729428</v>
       </c>
       <c r="F10" s="5">
-        <v>154769.0</v>
+        <v>154769</v>
       </c>
       <c r="G10" s="5">
-        <v>6573534.0</v>
+        <v>6573534</v>
       </c>
       <c r="H10" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I10" s="5">
-        <v>1.0816332E7</v>
+        <v>10816332</v>
       </c>
       <c r="J10" s="5">
-        <v>-4342797.0</v>
+        <v>-4342797</v>
       </c>
       <c r="K10" s="5">
-        <v>1125.0</v>
+        <v>1125</v>
       </c>
       <c r="L10" s="5">
-        <v>6573534.0</v>
+        <v>6573534</v>
       </c>
       <c r="M10" s="5">
-        <v>6729428.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>6729428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44286.0</v>
+        <v>44286</v>
       </c>
       <c r="B11" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>7054816.205479452</v>
+        <v>7054816.2054794524</v>
       </c>
       <c r="D11" s="5">
-        <v>268071.5342465754</v>
+        <v>268071.53424657538</v>
       </c>
       <c r="E11" s="5">
         <v>7322888.493150685</v>
@@ -785,83 +826,83 @@
         <v>165132.56164383562</v>
       </c>
       <c r="G11" s="5">
-        <v>7156630.684931506</v>
+        <v>7156630.6849315064</v>
       </c>
       <c r="H11" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I11" s="5">
-        <v>1.2007327890410958E7</v>
+        <v>12007327.890410958</v>
       </c>
       <c r="J11" s="5">
-        <v>-4950696.205479452</v>
+        <v>-4950696.2054794524</v>
       </c>
       <c r="K11" s="5">
-        <v>1125.0</v>
+        <v>1125</v>
       </c>
       <c r="L11" s="5">
-        <v>7156630.684931506</v>
+        <v>7156630.6849315064</v>
       </c>
       <c r="M11" s="5">
         <v>7322888.493150685</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44377.0</v>
+        <v>44377</v>
       </c>
       <c r="B12" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5">
-        <v>7588898.446575343</v>
+        <v>7588898.4465753427</v>
       </c>
       <c r="D12" s="5">
         <v>334044.04109589045</v>
       </c>
       <c r="E12" s="5">
-        <v>7922942.991780822</v>
+        <v>7922942.9917808222</v>
       </c>
       <c r="F12" s="5">
         <v>175611.27397260274</v>
       </c>
       <c r="G12" s="5">
-        <v>7746206.221917808</v>
+        <v>7746206.2219178081</v>
       </c>
       <c r="H12" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I12" s="5">
-        <v>1.321155706849315E7</v>
+        <v>13211557.06849315</v>
       </c>
       <c r="J12" s="5">
-        <v>-5565349.846575342</v>
+        <v>-5565349.8465753421</v>
       </c>
       <c r="K12" s="5">
-        <v>1125.0</v>
+        <v>1125</v>
       </c>
       <c r="L12" s="5">
-        <v>7746206.221917808</v>
+        <v>7746206.2219178081</v>
       </c>
       <c r="M12" s="5">
-        <v>7922942.991780822</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>7922942.9917808222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44469.0</v>
+        <v>44469</v>
       </c>
       <c r="B13" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5">
-        <v>8128849.723287672</v>
+        <v>8128849.7232876718</v>
       </c>
       <c r="D13" s="5">
-        <v>400741.5205479452</v>
+        <v>400741.52054794523</v>
       </c>
       <c r="E13" s="5">
-        <v>8529591.49589041</v>
+        <v>8529591.4958904106</v>
       </c>
       <c r="F13" s="5">
         <v>186205.13698630137</v>
@@ -870,311 +911,399 @@
         <v>8342260.610958904</v>
       </c>
       <c r="H13" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I13" s="5">
-        <v>1.4429019534246575E7</v>
+        <v>14429019.534246575</v>
       </c>
       <c r="J13" s="5">
-        <v>-6186757.923287671</v>
+        <v>-6186757.9232876711</v>
       </c>
       <c r="K13" s="5">
-        <v>1125.0</v>
+        <v>1125</v>
       </c>
       <c r="L13" s="5">
         <v>8342260.610958904</v>
       </c>
       <c r="M13" s="5">
-        <v>8529591.49589041</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>8529591.4958904106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>44561.0</v>
+        <v>44561</v>
       </c>
       <c r="B14" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5">
-        <v>8668801.0</v>
+        <v>8668801</v>
       </c>
       <c r="D14" s="5">
-        <v>467439.0</v>
+        <v>467439</v>
       </c>
       <c r="E14" s="5">
-        <v>9136240.0</v>
+        <v>9136240</v>
       </c>
       <c r="F14" s="5">
-        <v>196799.0</v>
+        <v>196799</v>
       </c>
       <c r="G14" s="5">
-        <v>8938315.0</v>
+        <v>8938315</v>
       </c>
       <c r="H14" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I14" s="5">
-        <v>1.5646482E7</v>
+        <v>15646482</v>
       </c>
       <c r="J14" s="5">
-        <v>-6808166.0</v>
+        <v>-6808166</v>
       </c>
       <c r="K14" s="5">
-        <v>1125.0</v>
+        <v>1125</v>
       </c>
       <c r="L14" s="5">
-        <v>8938315.0</v>
+        <v>8938315</v>
       </c>
       <c r="M14" s="5">
-        <v>9136240.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>9136240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>44651.0</v>
+        <v>44651</v>
       </c>
       <c r="B15" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C15" s="5">
-        <v>8360675.273972603</v>
+        <v>8360675.2739726026</v>
       </c>
       <c r="D15" s="5">
-        <v>973527.493150685</v>
+        <v>973527.49315068498</v>
       </c>
       <c r="E15" s="5">
         <v>9334203.01369863</v>
       </c>
       <c r="F15" s="5">
-        <v>595718.9452054795</v>
+        <v>595718.94520547951</v>
       </c>
       <c r="G15" s="5">
-        <v>8737286.808219178</v>
+        <v>8737286.8082191776</v>
       </c>
       <c r="H15" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I15" s="5">
-        <v>1.5311537753424658E7</v>
+        <v>15311537.753424658</v>
       </c>
       <c r="J15" s="5">
-        <v>-6674249.94520548</v>
+        <v>-6674249.9452054799</v>
       </c>
       <c r="K15" s="5">
         <v>1196.013698630137</v>
       </c>
       <c r="L15" s="5">
-        <v>8737286.808219178</v>
+        <v>8737286.8082191776</v>
       </c>
       <c r="M15" s="5">
         <v>9334203.01369863</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>44742.0</v>
+        <v>44742</v>
       </c>
       <c r="B16" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C16" s="5">
-        <v>8049125.928767123</v>
+        <v>8049125.9287671233</v>
       </c>
       <c r="D16" s="5">
-        <v>1485239.191780822</v>
+        <v>1485239.1917808219</v>
       </c>
       <c r="E16" s="5">
-        <v>9534365.616438355</v>
+        <v>9534365.6164383553</v>
       </c>
       <c r="F16" s="5">
-        <v>999071.3342465754</v>
+        <v>999071.33424657537</v>
       </c>
       <c r="G16" s="5">
-        <v>8534024.969863014</v>
+        <v>8534024.9698630143</v>
       </c>
       <c r="H16" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I16" s="5">
-        <v>1.497287190410959E7</v>
+        <v>14972871.90410959</v>
       </c>
       <c r="J16" s="5">
-        <v>-6538845.934246575</v>
+        <v>-6538845.9342465755</v>
       </c>
       <c r="K16" s="5">
         <v>1267.8164383561643</v>
       </c>
       <c r="L16" s="5">
-        <v>8534024.969863014</v>
+        <v>8534024.9698630143</v>
       </c>
       <c r="M16" s="5">
-        <v>9534365.616438355</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>9534365.6164383553</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>44834.0</v>
+        <v>44834</v>
       </c>
       <c r="B17" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C17" s="5">
-        <v>7734152.964383561</v>
+        <v>7734152.9643835612</v>
       </c>
       <c r="D17" s="5">
-        <v>2002574.095890411</v>
+        <v>2002574.0958904109</v>
       </c>
       <c r="E17" s="5">
-        <v>9736727.808219178</v>
+        <v>9736727.8082191776</v>
       </c>
       <c r="F17" s="5">
         <v>1406856.1671232877</v>
       </c>
       <c r="G17" s="5">
-        <v>8328529.484931507</v>
+        <v>8328529.4849315071</v>
       </c>
       <c r="H17" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I17" s="5">
-        <v>1.4630484452054795E7</v>
+        <v>14630484.452054795</v>
       </c>
       <c r="J17" s="5">
-        <v>-6401953.967123288</v>
+        <v>-6401953.9671232877</v>
       </c>
       <c r="K17" s="5">
         <v>1340.4082191780822</v>
       </c>
       <c r="L17" s="5">
-        <v>8328529.484931507</v>
+        <v>8328529.4849315071</v>
       </c>
       <c r="M17" s="5">
-        <v>9736727.808219178</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>9736727.8082191776</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>44926.0</v>
+        <v>44926</v>
       </c>
       <c r="B18" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C18" s="5">
-        <v>7419180.0</v>
+        <v>7419180</v>
       </c>
       <c r="D18" s="5">
-        <v>2519909.0</v>
+        <v>2519909</v>
       </c>
       <c r="E18" s="5">
-        <v>9939090.0</v>
+        <v>9939090</v>
       </c>
       <c r="F18" s="5">
-        <v>1814641.0</v>
+        <v>1814641</v>
       </c>
       <c r="G18" s="5">
-        <v>8123034.0</v>
+        <v>8123034</v>
       </c>
       <c r="H18" s="5">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="I18" s="5">
-        <v>1.4288097E7</v>
+        <v>14288097</v>
       </c>
       <c r="J18" s="5">
-        <v>-6265062.0</v>
+        <v>-6265062</v>
       </c>
       <c r="K18" s="5">
-        <v>1413.0</v>
+        <v>1413</v>
       </c>
       <c r="L18" s="5">
-        <v>8123034.0</v>
+        <v>8123034</v>
       </c>
       <c r="M18" s="5">
-        <v>9939090.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>9939090</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <v>45016.0</v>
+        <v>45016</v>
       </c>
       <c r="B19" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-    </row>
-    <row r="20">
+        <v>3</v>
+      </c>
+      <c r="C19" s="8">
+        <v>7039959.2054794515</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2495011.3013698631</v>
+      </c>
+      <c r="E19" s="8">
+        <v>10274697.287671233</v>
+      </c>
+      <c r="F19" s="8">
+        <v>2214226.6986301374</v>
+      </c>
+      <c r="G19" s="8">
+        <v>8059055.5890410962</v>
+      </c>
+      <c r="H19" s="8">
+        <v>100000</v>
+      </c>
+      <c r="I19" s="8">
+        <v>13063879.767123288</v>
+      </c>
+      <c r="J19" s="8">
+        <v>-5104823.4246575339</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1413</v>
+      </c>
+      <c r="L19" s="8">
+        <v>8059055.5890410962</v>
+      </c>
+      <c r="M19" s="8">
+        <v>10274697.287671233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>45107.0</v>
+        <v>45107</v>
       </c>
       <c r="B20" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-    </row>
-    <row r="21">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8">
+        <v>6656524.8465753421</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2469836.9616438355</v>
+      </c>
+      <c r="E20" s="8">
+        <v>10614033.545205479</v>
+      </c>
+      <c r="F20" s="8">
+        <v>2618252.2383561647</v>
+      </c>
+      <c r="G20" s="8">
+        <v>7994366.3068493148</v>
+      </c>
+      <c r="H20" s="8">
+        <v>100000</v>
+      </c>
+      <c r="I20" s="8">
+        <v>11826060.120547945</v>
+      </c>
+      <c r="J20" s="8">
+        <v>-3931693.3095890409</v>
+      </c>
+      <c r="K20" s="8">
+        <v>1413</v>
+      </c>
+      <c r="L20" s="8">
+        <v>7994366.3068493148</v>
+      </c>
+      <c r="M20" s="8">
+        <v>10614033.545205479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>45199.0</v>
+        <v>45199</v>
       </c>
       <c r="B21" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-    </row>
-    <row r="22">
+        <v>3</v>
+      </c>
+      <c r="C21" s="8">
+        <v>6268876.9232876711</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2444385.9808219178</v>
+      </c>
+      <c r="E21" s="8">
+        <v>10957098.772602741</v>
+      </c>
+      <c r="F21" s="8">
+        <v>3026717.6191780823</v>
+      </c>
+      <c r="G21" s="8">
+        <v>7928966.1534246579</v>
+      </c>
+      <c r="H21" s="8">
+        <v>100000</v>
+      </c>
+      <c r="I21" s="8">
+        <v>10574638.060273971</v>
+      </c>
+      <c r="J21" s="8">
+        <v>-2745671.6547945207</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1413</v>
+      </c>
+      <c r="L21" s="8">
+        <v>7928966.1534246579</v>
+      </c>
+      <c r="M21" s="8">
+        <v>10957098.772602741</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>45291.0</v>
+        <v>45291</v>
       </c>
       <c r="B22" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-    </row>
-    <row r="23">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7">
+        <v>5881229</v>
+      </c>
+      <c r="D22" s="7">
+        <v>2418935</v>
+      </c>
+      <c r="E22" s="7">
+        <v>11300164</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3435183</v>
+      </c>
+      <c r="G22" s="7">
+        <v>7863566</v>
+      </c>
+      <c r="H22" s="7">
+        <v>100000</v>
+      </c>
+      <c r="I22" s="7">
+        <v>9323216</v>
+      </c>
+      <c r="J22" s="7">
+        <v>-1559650</v>
+      </c>
+      <c r="K22" s="7">
+        <v>1413</v>
+      </c>
+      <c r="L22" s="7">
+        <v>7863566</v>
+      </c>
+      <c r="M22" s="7">
+        <v>11300164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>45382.0</v>
+        <v>45382</v>
       </c>
       <c r="B23" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1188,12 +1317,12 @@
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>45473.0</v>
+        <v>45473</v>
       </c>
       <c r="B24" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1207,12 +1336,12 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>45565.0</v>
+        <v>45565</v>
       </c>
       <c r="B25" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1227,9 +1356,7 @@
       <c r="M25" s="7"/>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>